<commit_message>
Updated Documentation for V1.0 Release
</commit_message>
<xml_diff>
--- a/Documentation/Willow_Joystick_BOM.xlsx
+++ b/Documentation/Willow_Joystick_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 24-12 Willow Joystick/Willow-Joystick/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="780" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017F6799-68B7-4DEE-82BF-40E5903B5C10}"/>
+  <xr:revisionPtr revIDLastSave="781" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1C2DDDE-FC4D-413C-BAC9-0CB5895B7A6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -1486,7 +1486,7 @@
   <dimension ref="A1:N93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="68">
-        <v>45709</v>
+        <v>45723</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>